<commit_message>
Included LTRs, refactored ERV IDs - standard nomeclatuture
</commit_message>
<xml_diff>
--- a/tabular/erv/erv-locus-data.xlsx
+++ b/tabular/erv/erv-locus-data.xlsx
@@ -8,20 +8,31 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/Retrovirus/Deltaretrovirus-GLUE/tabular/erv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD3C467A-1E07-BF41-8FA5-49921045929D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F4AE9AE-8E57-7F4C-B2A4-3C144C976A3D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22400" yWindow="2500" windowWidth="27600" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21700" yWindow="2460" windowWidth="27600" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="query_result" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="63">
   <si>
     <t>record_ID</t>
   </si>
@@ -29,18 +40,6 @@
     <t>organism</t>
   </si>
   <si>
-    <t>target_datatype</t>
-  </si>
-  <si>
-    <t>target_version</t>
-  </si>
-  <si>
-    <t>target_name</t>
-  </si>
-  <si>
-    <t>probe_type</t>
-  </si>
-  <si>
     <t>scaffold</t>
   </si>
   <si>
@@ -62,21 +61,6 @@
     <t>Miniopterus_natalensis</t>
   </si>
   <si>
-    <t>low_coverage</t>
-  </si>
-  <si>
-    <t>Mnat.v1</t>
-  </si>
-  <si>
-    <t>291302_ref_Mnat.v1_chrUn.fa</t>
-  </si>
-  <si>
-    <t>ORF</t>
-  </si>
-  <si>
-    <t>gi|1016328890|ref|NW_015504317.1|</t>
-  </si>
-  <si>
     <t>GTNCTCCCGCTCGCACAAGCCCTTTCCCGAGGCCTCTTACGGGTCCAGCCTCTACAATCCCTTTGCCTATTAGCCCCGCTTAAGTCCTCACAGGTATCAAGCCACAGCAGCCATTCTTTTGAGGAGGAGCTGGATGAAGCTGAAGGGCCCTCCATGGAGGGGCAAGAAGAAGGAAGTCAGAGCAGACAGCGGAAACCGAAGGAGCCATGA</t>
   </si>
   <si>
@@ -89,12 +73,6 @@
     <t>Miniopterus_schreibersii</t>
   </si>
   <si>
-    <t>MinSch_v1</t>
-  </si>
-  <si>
-    <t>GCA_004026525.1_MinSch_v1_BIUU_genomic.fna</t>
-  </si>
-  <si>
     <t>ATGGGACAAGGGTCGAGTCACCTCCTAAATCAGGTCCCTCGGGGCCTTACTTATACCCAGTGGGAATCTCTCCTTCTGGCCTCTCGCACACTCTCTCCTCGACCCTCCGACTCGGACATTAAGACTCTCAGACGTTTCTTAAAGGTTTTCCTCCCGAAGAATCCTTGGCCCTTACGACCATCACAGGCTTGGGTTGACTCTATTCACCCAACACCACCGGGCCGAGTCCGAGAGATG</t>
   </si>
   <si>
@@ -113,15 +91,6 @@
     <t>Murina_aurata_feae</t>
   </si>
   <si>
-    <t>MurFea_v1</t>
-  </si>
-  <si>
-    <t>GCA_004026665.1_MurFea_v1_BIUU_genomic.fna</t>
-  </si>
-  <si>
-    <t>PVJC01054996.1</t>
-  </si>
-  <si>
     <t>TCTTCCCTTCTCCTTTCCGAGGTCCCCCGGGGCCTCGATTTCAATTCCTGGACGGACCTCCTCCGTGCCAGTCGCACTCTTACGCCTGGCCCTACAAACGGGGACATTCTTGCTTTACGCAAATTTCTTAAAAAATTCTTACCTTTTAATTCGTGGCCCGCGATCATCACGACATCCTGGGTCACCTCTATTACTCCTTCTCCTCCGGGCCGCGTTAAGGAGATC</t>
   </si>
   <si>
@@ -134,15 +103,6 @@
     <t>Platanista_minor</t>
   </si>
   <si>
-    <t>PlaMin_v1_BIUU</t>
-  </si>
-  <si>
-    <t>GCA_004363435.1_PlaMin_v1_BIUU_genomic.fna</t>
-  </si>
-  <si>
-    <t>RJWK010047772.1</t>
-  </si>
-  <si>
     <t>ATGGGTAACTCCCAATCCCATTATAAACAACCAGGAACCATTAATCCATCTGAATGGCTAAATTTATTACAGGCAGCTCAAAAATTAAATCCTGGTCCATCTGATTATGATATCAAACTTCTGCGCCGCTTTTGTAGGGATTGGGAGAGACGAAACCAAGAGCCTTGGCGGTATCGTTTTCCCGCTGCCAAAGACTGCCCACGCGAGAAATATGGGCGTACACAGCAAATTCTTAATATCCTAGATGCTGCCTTAAAACCTAAGGATGCAACAGACCCACCCCCCCTTGAGCCTATCACCCCTCAGACTTCACCTCCCAACCCTCTGGCTAAGGAACCCCTTGTCAACACCCCTGAGCCACCGCCCCCTTACAATCCTCCCGGGGCATCTGCACCCCCTACCTTGCTCCCTGTTGTTCATGAACCCGGCGGGAATCCACCTCGCCATCGCCCCTGGACCCTCAAAGAACTCCATGATTTTAAACGAGAGGTCGAAGGGAAGGCCCCGGGTTCCACTCCCTGGAATCAGTCCCTCCGCCTGATCCTTGACCAGGCGGATCCTTCCCCATCTGATCTGAACCAGCTCTCCGACTATCTCTGTACTCCTGTTGACCGTACTGCACACACTGCCGCGGTCGCTGCTGTCGTGGCCCGGGCTGAACAGGATAGTCAAATCCCGGGGTATAACCCTGAAGCCGGCCCGCTTCATGTGCAGGCCAACAACCCTCTCAATCAGGGCCTCCGAAGAGAGTTCCAGCGAATATGGCTGGCAGCATGGCGAGATTTACCCACAAGCCCCTTAGTCCAGCCCTGGTCGACCATTACTCAGGGTCCGGCCGAGCCTTACACTGATTTCATTAATCGTCTCCAGGCCGCCTTGTTGGACAACCTTCCAGATGGGATACCTTCTGGACCCATTCTTGATTCCTTGAGCTATATAAATGCCAATAAGGATTGCCAACAGGTCCTCGTCAGCCGAGGTCTCCAAAATGCCCCTGTTGATCAAAAATTACGCGCCTGTGCCCATTGGGGTCCCAAGGCTAAGGCAGCTACAGTTTTGGTCCAGAGGGTGACCCCTGGACCCCCGAAGACACGCCTCCCTCCCGGTCCCTGCTACCGCTGCAACAAGGAGGGTCATTGGTCTAAAGAATGTCCCCTCAAGCCTAAGGCTCCCCCTGGCCACTGACCCCTTTGTGGAAATGCCACCCATTGGAAACGGGACTGCCCTCTTAACTCTCGGGCCCCAAAAAACTAGATCGGGGGGGCCACCATACCC</t>
   </si>
   <si>
@@ -164,14 +124,110 @@
     <t>ERV-Delta.3-Murina_aurata</t>
   </si>
   <si>
-    <t>ERV-Delta.1-Platanista_minor</t>
+    <t>ERV-Delta.6-Platanista_minor</t>
+  </si>
+  <si>
+    <t>PJEU01009902</t>
+  </si>
+  <si>
+    <t>PJEM01004257</t>
+  </si>
+  <si>
+    <t>PISW01001682</t>
+  </si>
+  <si>
+    <t>PITD01006283</t>
+  </si>
+  <si>
+    <t>NKTL01022466</t>
+  </si>
+  <si>
+    <t>Cryptoprocta ferox</t>
+  </si>
+  <si>
+    <t>Helogale parvula</t>
+  </si>
+  <si>
+    <t>Mungos mungo</t>
+  </si>
+  <si>
+    <t>Suricata suricatta</t>
+  </si>
+  <si>
+    <t>Solenodon paradoxus</t>
+  </si>
+  <si>
+    <t>LDJU01000221</t>
+  </si>
+  <si>
+    <t>LVEH01002092</t>
+  </si>
+  <si>
+    <t>PVLB01015338</t>
+  </si>
+  <si>
+    <t>PVKU01000816</t>
+  </si>
+  <si>
+    <t>Hipposideros galeritus</t>
+  </si>
+  <si>
+    <t>Anoura caudifer</t>
+  </si>
+  <si>
+    <t>Rhinolophus sinicus</t>
+  </si>
+  <si>
+    <t>RJWK010047772</t>
+  </si>
+  <si>
+    <t>PVJC01054996</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>ERV-Delta.2-Rhinolophus_sinicus</t>
+  </si>
+  <si>
+    <t>ERV-Delta.4-Hipposideros_galeritus</t>
+  </si>
+  <si>
+    <t>Miniopterus natalensis</t>
+  </si>
+  <si>
+    <t>Miniopterus schreibersii</t>
+  </si>
+  <si>
+    <t>Murina aurata feae</t>
+  </si>
+  <si>
+    <t>Platanista minor</t>
+  </si>
+  <si>
+    <t>ERV-Delta.5-Anoura_caudifer</t>
+  </si>
+  <si>
+    <t>ERV-Delta.7-Cryptoprocta_ferox</t>
+  </si>
+  <si>
+    <t>ERV-Delta.7-Helogale_parvula</t>
+  </si>
+  <si>
+    <t>ERV-Delta.7-Mungos_mungo</t>
+  </si>
+  <si>
+    <t>ERV-Delta.7-Suricata_suricatta</t>
+  </si>
+  <si>
+    <t>ERV-Delta.8-Solenodon_paradoxus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -306,8 +362,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="34">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -491,6 +562,18 @@
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59996337778862885"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -654,7 +737,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -662,6 +745,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1018,226 +1119,364 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="A1:M5"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="39.83203125" customWidth="1"/>
     <col min="2" max="2" width="18.33203125" customWidth="1"/>
-    <col min="3" max="3" width="25.83203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="18.5" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="11"/>
+    <col min="8" max="8" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="7">
+        <v>1783</v>
+      </c>
+      <c r="C2" s="7">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="6">
+        <v>685870</v>
+      </c>
+      <c r="F2" s="6">
+        <v>688987</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="7">
+        <v>1587</v>
+      </c>
+      <c r="C3" s="7">
+        <v>1</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="6">
+        <v>503</v>
+      </c>
+      <c r="F3" s="6">
+        <v>2089</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="7">
+        <v>661</v>
+      </c>
+      <c r="C4" s="7">
+        <v>2</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="E4" s="6">
+        <v>224</v>
+      </c>
+      <c r="F4" s="6">
+        <v>884</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="7">
+        <v>2571</v>
+      </c>
+      <c r="C5" s="7">
+        <v>3</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="5">
+        <v>2991</v>
+      </c>
+      <c r="F5" s="5">
+        <v>9624</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="7">
+        <v>606</v>
+      </c>
+      <c r="C6" s="7">
+        <v>4</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="E6" s="6">
+        <v>37283</v>
+      </c>
+      <c r="F6" s="6">
+        <v>37888</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="7">
+        <v>261</v>
+      </c>
+      <c r="C7" s="7">
         <v>5</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="D7" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="6">
+        <v>300731</v>
+      </c>
+      <c r="F7" s="6">
+        <v>300991</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="7">
+        <v>4522</v>
+      </c>
+      <c r="C8" s="7">
         <v>6</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="D8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="5">
+        <v>2710</v>
+      </c>
+      <c r="F8" s="5">
+        <v>10772</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" s="7">
+        <v>636</v>
+      </c>
+      <c r="C9" s="7">
         <v>7</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="D9" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="6">
+        <v>63280</v>
+      </c>
+      <c r="F9" s="6">
+        <v>63915</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="7">
+        <v>551</v>
+      </c>
+      <c r="C10" s="7">
+        <v>7</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="6">
+        <v>95137</v>
+      </c>
+      <c r="F10" s="6">
+        <v>95687</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="7">
+        <v>535</v>
+      </c>
+      <c r="C11" s="7">
+        <v>7</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="6">
+        <v>85328</v>
+      </c>
+      <c r="F11" s="6">
+        <v>85862</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="7">
+        <v>552</v>
+      </c>
+      <c r="C12" s="7">
+        <v>7</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="6">
+        <v>94127</v>
+      </c>
+      <c r="F12" s="6">
+        <v>94678</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="7">
+        <v>591</v>
+      </c>
+      <c r="C13" s="7">
         <v>8</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="3">
-        <v>1783</v>
-      </c>
-      <c r="C2" s="3">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>2310068</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2">
-        <v>686392</v>
-      </c>
-      <c r="L2">
-        <v>688174</v>
-      </c>
-      <c r="M2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="3">
-        <v>1587</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>2310072</v>
-      </c>
-      <c r="E3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K3">
-        <v>503</v>
-      </c>
-      <c r="L3">
-        <v>2089</v>
-      </c>
-      <c r="M3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" s="3">
-        <v>2571</v>
-      </c>
-      <c r="C4" s="3">
-        <v>3</v>
-      </c>
-      <c r="D4">
-        <v>2670881</v>
-      </c>
-      <c r="E4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" t="s">
-        <v>31</v>
-      </c>
-      <c r="I4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" t="s">
-        <v>32</v>
-      </c>
-      <c r="K4">
-        <v>4686</v>
-      </c>
-      <c r="L4">
-        <v>7256</v>
-      </c>
-      <c r="M4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" s="3">
-        <v>4522</v>
-      </c>
-      <c r="C5" s="3">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>2713584</v>
-      </c>
-      <c r="E5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" t="s">
-        <v>39</v>
-      </c>
-      <c r="K5">
-        <v>4226</v>
-      </c>
-      <c r="L5">
-        <v>8747</v>
-      </c>
-      <c r="M5" t="s">
-        <v>19</v>
+      <c r="D13" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="6">
+        <v>630</v>
+      </c>
+      <c r="F13" s="6">
+        <v>1220</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H13">
+    <sortCondition ref="C2:C13"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1260,139 +1499,139 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B2">
         <v>1621115</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>2310068</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>1621104</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B5">
         <v>1621105</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <v>1621106</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B7">
         <v>1621107</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B8">
         <v>2310072</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B9">
         <v>1621109</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B10">
         <v>2670881</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B11">
         <v>2310176</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B12">
         <v>2577530</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B13">
         <v>2713584</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>